<commit_message>
2 nieuwe logs toegevoegd (44 en 45)aan het logbestand.
</commit_message>
<xml_diff>
--- a/Logboek IC-INf-1D SunnySocks.xlsx
+++ b/Logboek IC-INf-1D SunnySocks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newuniversity-my.sharepoint.com/personal/dinand_rengers_student_nhlstenden_com/Documents/Dinand Rengers NHLStenden/Periode 1/Project SunnySocks IC-INF-1D/Bestanden/Project SunnySocks/SunnySocks/SunnySocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newuniversity-my.sharepoint.com/personal/dinand_rengers_student_nhlstenden_com/Documents/Dinand Rengers NHLStenden/Periode 1/Project SunnySocks IC-INF-1D/Bestanden/Project SunnySocks/SunnySocks/SunnySocks-P1-IC-INF-1D/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCA1129A-32F2-4E7B-9B8E-5D7E95481542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{CCA1129A-32F2-4E7B-9B8E-5D7E95481542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20CF2BEF-603C-4041-9D27-A4B9FCEF37EC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{A0DF4751-B08E-4820-988C-0E0B1DC12E30}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15435" xr2:uid="{A0DF4751-B08E-4820-988C-0E0B1DC12E30}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="182">
   <si>
     <t>Logbestand - IC-INF-1D</t>
   </si>
@@ -555,6 +555,33 @@
   </si>
   <si>
     <t>43</t>
+  </si>
+  <si>
+    <t>4ecce020</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>PascalWesterhof</t>
+  </si>
+  <si>
+    <t>11-10-2024, 13.34</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Basis aangelegd voor blog pagina en header hieraan toegevoegd.</t>
+  </si>
+  <si>
+    <t>Heb een logboek aangemaakt voor onze logs, en heb mijn overons pagina bijna afgemaakt. Ook heb ik wat extra informatie bij de style guide en de README.</t>
+  </si>
+  <si>
+    <t>59b8e48f</t>
+  </si>
+  <si>
+    <t>11-10-2024, 15.56</t>
   </si>
 </sst>
 </file>
@@ -928,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F91A9F-A548-428B-BA55-74F0531AC96F}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="F56" sqref="F55:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,6 +1749,40 @@
         <v>131</v>
       </c>
     </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>